<commit_message>
Initial CPQ Flask App with Agentic AI pipeline and performance comparison
</commit_message>
<xml_diff>
--- a/outputs/test_results_2025-04-20.xlsx
+++ b/outputs/test_results_2025-04-20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,11 +472,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Perez-Smith</t>
+          <t>Stephens PLC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,26 +486,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Desktop</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>2488</v>
+        <v>3000</v>
       </c>
       <c r="G2" t="n">
-        <v>27368</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Perez-Smith</t>
+          <t>Stephens PLC</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -519,198 +519,140 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>3000</v>
       </c>
       <c r="G3" t="n">
-        <v>24000</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Perez-Smith</t>
+          <t>Stephens PLC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hardware</t>
+          <t>Software</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Switch</t>
+          <t>Office 365</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G4" t="n">
-        <v>500</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Perez-Smith</t>
+          <t>Stephens PLC</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hardware</t>
+          <t>Software</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Firewall</t>
+          <t>Service pack</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F5" t="n">
         <v>100</v>
       </c>
       <c r="G5" t="n">
-        <v>600</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Perez-Smith</t>
+          <t>Stephens PLC</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Labor</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>H/W setup</t>
+          <t>Router</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G6" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Perez-Smith</t>
+          <t>Stephens PLC</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MS 365</t>
+          <t>Desktop</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>150</v>
+        <v>2488</v>
       </c>
       <c r="G7" t="n">
-        <v>1950</v>
+        <v>24880</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>101</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Perez-Smith</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Hardware</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Laptop</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3000</v>
-      </c>
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>101</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Perez-Smith</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Software</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Antivirus</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" t="n">
-        <v>60</v>
-      </c>
-      <c r="G9" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>128796</v>
+        <v>69080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>